<commit_message>
ui and server updated, almost done
</commit_message>
<xml_diff>
--- a/relacionales.xlsx
+++ b/relacionales.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\dataleik\demo_tienda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95052C16-1626-471B-A5DD-B9D7A849DF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC55411-B2C5-4142-B67D-A00D21F27F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categorias_id" sheetId="2" r:id="rId1"/>
     <sheet name="productos_id" sheetId="4" r:id="rId2"/>
-    <sheet name="usuarios registrados" sheetId="5" r:id="rId3"/>
+    <sheet name="usuarios_registrados" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE25D005-717B-4082-AC84-24FE3AE30F4A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEF39BD-1E87-41B7-94CA-3C5C88DB3D13}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>